<commit_message>
Funcional despues de cambios en clases
</commit_message>
<xml_diff>
--- a/src/test/resources/archivos/archivo.xlsx
+++ b/src/test/resources/archivos/archivo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
   <si>
     <t>Documento</t>
   </si>
@@ -131,7 +131,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -269,6 +269,160 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>